<commit_message>
added multilingual, wrong vocab and ambigous  test cases and improved the evaluation framework
</commit_message>
<xml_diff>
--- a/EvaluationAndTesting/Evaluation/EvaluationReport.xlsx
+++ b/EvaluationAndTesting/Evaluation/EvaluationReport.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5424" uniqueCount="4029">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5420" uniqueCount="4026">
   <si>
     <t>Metric</t>
   </si>
@@ -13618,16 +13618,6 @@
 * **Specialization:**  The division of labor and production</t>
   </si>
   <si>
-    <t>How does inflation affect prices, GDP, employment, and interest rates in a country like the USA during a recession caused by external shocks?</t>
-  </si>
-  <si>
-    <t>Could you provide more details on what you are asking about?</t>
-  </si>
-  <si>
-    <t>During a recession in the USA caused by external shocks, inflation's impact on prices, GDP, employment, and interest rates is complex and depends on the specific nature of the shock.  Generally, a recession stemming from external shocks (e.g., supply chain disruptions, geopolitical instability) tends to be associated with *stagflation* – a combination of slow economic growth (or even contraction) and rising prices.
-* **Prices:**  Prices will likely rise due to supply-side pressures</t>
-  </si>
-  <si>
     <t>Is the gold standard still used today?</t>
   </si>
   <si>
@@ -13821,25 +13811,13 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
   <numFmts count="0"/>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
@@ -13856,7 +13834,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -13886,26 +13864,11 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="8">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -13916,7 +13879,7 @@
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general"/>
     </xf>
-    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
@@ -13925,13 +13888,7 @@
     <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="3" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="3" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
@@ -14236,7 +14193,7 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:I1353"/>
+  <dimension ref="A1:I1352"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="1"/>
   </sheetViews>
@@ -14254,35 +14211,35 @@
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="C1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D1" s="8" t="s">
+      <c r="D1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="8" t="s">
+      <c r="E1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="8" t="s">
+      <c r="F1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="8" t="s">
+      <c r="G1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="8" t="s">
+      <c r="H1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="7" t="s">
+      <c r="I1" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="16.5">
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
       <c r="A2" s="3" t="s">
         <v>11</v>
       </c>
@@ -14311,7 +14268,7 @@
         <v>14</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="16.5">
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75">
       <c r="A3" s="3" t="s">
         <v>15</v>
       </c>
@@ -14340,7 +14297,7 @@
         <v>14</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="16.5">
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75">
       <c r="A4" s="3" t="s">
         <v>18</v>
       </c>
@@ -14369,7 +14326,7 @@
         <v>21</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="16.5">
+    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75">
       <c r="A5" s="3" t="s">
         <v>22</v>
       </c>
@@ -14398,7 +14355,7 @@
         <v>14</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="16.5">
+    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18.75">
       <c r="A6" s="3" t="s">
         <v>25</v>
       </c>
@@ -14414,7 +14371,7 @@
       <c r="E6" s="4">
         <v>0.9230769181065088</v>
       </c>
-      <c r="F6" s="9">
+      <c r="F6" s="7">
         <v>1</v>
       </c>
       <c r="G6" s="4">
@@ -14427,7 +14384,7 @@
         <v>14</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="16.5">
+    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="18.75">
       <c r="A7" s="3" t="s">
         <v>28</v>
       </c>
@@ -14443,10 +14400,10 @@
       <c r="E7" s="4">
         <v>0.9230769181065088</v>
       </c>
-      <c r="F7" s="9">
+      <c r="F7" s="7">
         <v>1</v>
       </c>
-      <c r="G7" s="9">
+      <c r="G7" s="7">
         <v>1</v>
       </c>
       <c r="H7" s="4">
@@ -14456,7 +14413,7 @@
         <v>14</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="16.5">
+    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="18.75">
       <c r="A8" s="3" t="s">
         <v>31</v>
       </c>
@@ -14469,10 +14426,10 @@
       <c r="D8" s="4">
         <v>0.1647595763206482</v>
       </c>
-      <c r="E8" s="9">
+      <c r="E8" s="7">
         <v>0</v>
       </c>
-      <c r="F8" s="9">
+      <c r="F8" s="7">
         <v>0</v>
       </c>
       <c r="G8" s="4">
@@ -14485,7 +14442,7 @@
         <v>21</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="16.5">
+    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="18.75">
       <c r="A9" s="3" t="s">
         <v>34</v>
       </c>
@@ -14501,7 +14458,7 @@
       <c r="E9" s="4">
         <v>0.9473684160664821</v>
       </c>
-      <c r="F9" s="9">
+      <c r="F9" s="7">
         <v>1</v>
       </c>
       <c r="G9" s="4">
@@ -14514,7 +14471,7 @@
         <v>14</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="16.5">
+    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="18.75">
       <c r="A10" s="3" t="s">
         <v>37</v>
       </c>
@@ -14543,7 +14500,7 @@
         <v>14</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="16.5">
+    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="18.75">
       <c r="A11" s="3" t="s">
         <v>40</v>
       </c>
@@ -14572,7 +14529,7 @@
         <v>14</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="16.5">
+    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="18.75">
       <c r="A12" s="3" t="s">
         <v>43</v>
       </c>
@@ -14601,7 +14558,7 @@
         <v>14</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="16.5">
+    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="18.75">
       <c r="A13" s="3" t="s">
         <v>46</v>
       </c>
@@ -14630,7 +14587,7 @@
         <v>14</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="16.5">
+    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="18.75">
       <c r="A14" s="3" t="s">
         <v>49</v>
       </c>
@@ -14643,10 +14600,10 @@
       <c r="D14" s="4">
         <v>0.02519473992288113</v>
       </c>
-      <c r="E14" s="9">
+      <c r="E14" s="7">
         <v>0</v>
       </c>
-      <c r="F14" s="9">
+      <c r="F14" s="7">
         <v>0</v>
       </c>
       <c r="G14" s="4">
@@ -14659,7 +14616,7 @@
         <v>21</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="16.5">
+    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="18.75">
       <c r="A15" s="3" t="s">
         <v>52</v>
       </c>
@@ -14688,7 +14645,7 @@
         <v>14</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="16.5">
+    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="18.75">
       <c r="A16" s="3" t="s">
         <v>55</v>
       </c>
@@ -14717,7 +14674,7 @@
         <v>14</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="16.5">
+    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="18.75">
       <c r="A17" s="3" t="s">
         <v>58</v>
       </c>
@@ -14746,7 +14703,7 @@
         <v>14</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="16.5">
+    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="18.75">
       <c r="A18" s="3" t="s">
         <v>61</v>
       </c>
@@ -14775,7 +14732,7 @@
         <v>14</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="16.5">
+    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="18.75">
       <c r="A19" s="3" t="s">
         <v>64</v>
       </c>
@@ -14804,7 +14761,7 @@
         <v>14</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="16.5">
+    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="18.75">
       <c r="A20" s="3" t="s">
         <v>67</v>
       </c>
@@ -14833,7 +14790,7 @@
         <v>14</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="16.5">
+    <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="18.75">
       <c r="A21" s="3" t="s">
         <v>70</v>
       </c>
@@ -14862,7 +14819,7 @@
         <v>14</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="16.5">
+    <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="18.75">
       <c r="A22" s="3" t="s">
         <v>73</v>
       </c>
@@ -14891,7 +14848,7 @@
         <v>14</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="16.5">
+    <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="100.5">
       <c r="A23" s="3" t="s">
         <v>76</v>
       </c>
@@ -14920,7 +14877,7 @@
         <v>21</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="16.5">
+    <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="18.75">
       <c r="A24" s="3" t="s">
         <v>79</v>
       </c>
@@ -14949,7 +14906,7 @@
         <v>21</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="16.5">
+    <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="18.75">
       <c r="A25" s="3" t="s">
         <v>82</v>
       </c>
@@ -14978,7 +14935,7 @@
         <v>14</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="16.5">
+    <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="18.75">
       <c r="A26" s="3" t="s">
         <v>85</v>
       </c>
@@ -15007,7 +14964,7 @@
         <v>14</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="27" customHeight="1" ht="16.5">
+    <row x14ac:dyDescent="0.25" r="27" customHeight="1" ht="18.75">
       <c r="A27" s="3" t="s">
         <v>88</v>
       </c>
@@ -15036,7 +14993,7 @@
         <v>14</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="28" customHeight="1" ht="16.5">
+    <row x14ac:dyDescent="0.25" r="28" customHeight="1" ht="18.75">
       <c r="A28" s="3" t="s">
         <v>91</v>
       </c>
@@ -15065,7 +15022,7 @@
         <v>21</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="29" customHeight="1" ht="16.5">
+    <row x14ac:dyDescent="0.25" r="29" customHeight="1" ht="18.75">
       <c r="A29" s="3" t="s">
         <v>94</v>
       </c>
@@ -15078,10 +15035,10 @@
       <c r="D29" s="4">
         <v>0.0898442268371582</v>
       </c>
-      <c r="E29" s="9">
+      <c r="E29" s="7">
         <v>0</v>
       </c>
-      <c r="F29" s="9">
+      <c r="F29" s="7">
         <v>0</v>
       </c>
       <c r="G29" s="4">
@@ -15094,7 +15051,7 @@
         <v>21</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="30" customHeight="1" ht="16.5">
+    <row x14ac:dyDescent="0.25" r="30" customHeight="1" ht="18.75">
       <c r="A30" s="3" t="s">
         <v>97</v>
       </c>
@@ -15123,7 +15080,7 @@
         <v>14</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="31" customHeight="1" ht="16.5">
+    <row x14ac:dyDescent="0.25" r="31" customHeight="1" ht="18.75">
       <c r="A31" s="3" t="s">
         <v>100</v>
       </c>
@@ -15152,7 +15109,7 @@
         <v>14</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="32" customHeight="1" ht="16.5">
+    <row x14ac:dyDescent="0.25" r="32" customHeight="1" ht="18.75">
       <c r="A32" s="3" t="s">
         <v>103</v>
       </c>
@@ -15181,7 +15138,7 @@
         <v>14</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="33" customHeight="1" ht="16.5">
+    <row x14ac:dyDescent="0.25" r="33" customHeight="1" ht="18.75">
       <c r="A33" s="3" t="s">
         <v>106</v>
       </c>
@@ -15197,10 +15154,10 @@
       <c r="E33" s="4">
         <v>0.8888888839506174</v>
       </c>
-      <c r="F33" s="9">
+      <c r="F33" s="7">
         <v>1</v>
       </c>
-      <c r="G33" s="9">
+      <c r="G33" s="7">
         <v>1</v>
       </c>
       <c r="H33" s="4">
@@ -15210,7 +15167,7 @@
         <v>14</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="34" customHeight="1" ht="16.5">
+    <row x14ac:dyDescent="0.25" r="34" customHeight="1" ht="18.75">
       <c r="A34" s="3" t="s">
         <v>109</v>
       </c>
@@ -15239,7 +15196,7 @@
         <v>14</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="35" customHeight="1" ht="16.5">
+    <row x14ac:dyDescent="0.25" r="35" customHeight="1" ht="18.75">
       <c r="A35" s="3" t="s">
         <v>112</v>
       </c>
@@ -15249,7 +15206,7 @@
       <c r="C35" s="3" t="s">
         <v>114</v>
       </c>
-      <c r="D35" s="9">
+      <c r="D35" s="7">
         <v>1</v>
       </c>
       <c r="E35" s="4">
@@ -15261,14 +15218,14 @@
       <c r="G35" s="4">
         <v>0.9999992847442627</v>
       </c>
-      <c r="H35" s="9">
+      <c r="H35" s="7">
         <v>1</v>
       </c>
       <c r="I35" s="3" t="s">
         <v>14</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="36" customHeight="1" ht="16.5">
+    <row x14ac:dyDescent="0.25" r="36" customHeight="1" ht="18.75">
       <c r="A36" s="3" t="s">
         <v>115</v>
       </c>
@@ -15297,7 +15254,7 @@
         <v>21</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="37" customHeight="1" ht="16.5">
+    <row x14ac:dyDescent="0.25" r="37" customHeight="1" ht="69">
       <c r="A37" s="3" t="s">
         <v>118</v>
       </c>
@@ -15339,10 +15296,10 @@
       <c r="D38" s="4">
         <v>0.5353262424468994</v>
       </c>
-      <c r="E38" s="9">
+      <c r="E38" s="7">
         <v>0</v>
       </c>
-      <c r="F38" s="9">
+      <c r="F38" s="7">
         <v>0</v>
       </c>
       <c r="G38" s="4">
@@ -15397,10 +15354,10 @@
       <c r="D40" s="4">
         <v>0.1383679211139679</v>
       </c>
-      <c r="E40" s="9">
+      <c r="E40" s="7">
         <v>0</v>
       </c>
-      <c r="F40" s="9">
+      <c r="F40" s="7">
         <v>0</v>
       </c>
       <c r="G40" s="4">
@@ -15629,10 +15586,10 @@
       <c r="D48" s="4">
         <v>0.3500352501869202</v>
       </c>
-      <c r="E48" s="9">
+      <c r="E48" s="7">
         <v>0</v>
       </c>
-      <c r="F48" s="9">
+      <c r="F48" s="7">
         <v>0</v>
       </c>
       <c r="G48" s="4">
@@ -15687,10 +15644,10 @@
       <c r="D50" s="4">
         <v>0.3937190175056458</v>
       </c>
-      <c r="E50" s="9">
+      <c r="E50" s="7">
         <v>0</v>
       </c>
-      <c r="F50" s="9">
+      <c r="F50" s="7">
         <v>0</v>
       </c>
       <c r="G50" s="4">
@@ -16670,7 +16627,7 @@
       <c r="C84" s="3" t="s">
         <v>261</v>
       </c>
-      <c r="D84" s="9">
+      <c r="D84" s="7">
         <v>1</v>
       </c>
       <c r="E84" s="4">
@@ -16679,10 +16636,10 @@
       <c r="F84" s="4">
         <v>1.491668146240062e-154</v>
       </c>
-      <c r="G84" s="9">
+      <c r="G84" s="7">
         <v>1</v>
       </c>
-      <c r="H84" s="9">
+      <c r="H84" s="7">
         <v>1</v>
       </c>
       <c r="I84" s="3" t="s">
@@ -16934,10 +16891,10 @@
       <c r="D93" s="4">
         <v>0.2928739786148071</v>
       </c>
-      <c r="E93" s="9">
+      <c r="E93" s="7">
         <v>0</v>
       </c>
-      <c r="F93" s="9">
+      <c r="F93" s="7">
         <v>0</v>
       </c>
       <c r="G93" s="4">
@@ -17105,7 +17062,7 @@
       <c r="C99" s="3" t="s">
         <v>306</v>
       </c>
-      <c r="D99" s="9">
+      <c r="D99" s="7">
         <v>1</v>
       </c>
       <c r="E99" s="4">
@@ -17114,10 +17071,10 @@
       <c r="F99" s="4">
         <v>1.22133866975547e-77</v>
       </c>
-      <c r="G99" s="9">
+      <c r="G99" s="7">
         <v>1</v>
       </c>
-      <c r="H99" s="9">
+      <c r="H99" s="7">
         <v>1</v>
       </c>
       <c r="I99" s="3" t="s">
@@ -17485,10 +17442,10 @@
       <c r="D112" s="4">
         <v>0.3415774703025818</v>
       </c>
-      <c r="E112" s="9">
+      <c r="E112" s="7">
         <v>0</v>
       </c>
-      <c r="F112" s="9">
+      <c r="F112" s="7">
         <v>0</v>
       </c>
       <c r="G112" s="4">
@@ -18129,7 +18086,7 @@
       <c r="F134" s="4">
         <v>1.22133866975547e-77</v>
       </c>
-      <c r="G134" s="9">
+      <c r="G134" s="7">
         <v>1</v>
       </c>
       <c r="H134" s="4">
@@ -18152,10 +18109,10 @@
       <c r="D135" s="4">
         <v>0.4096087515354156</v>
       </c>
-      <c r="E135" s="9">
+      <c r="E135" s="7">
         <v>0</v>
       </c>
-      <c r="F135" s="9">
+      <c r="F135" s="7">
         <v>0</v>
       </c>
       <c r="G135" s="4">
@@ -18468,19 +18425,19 @@
       <c r="C146" s="3" t="s">
         <v>447</v>
       </c>
-      <c r="D146" s="9">
+      <c r="D146" s="7">
         <v>1</v>
       </c>
       <c r="E146" s="4">
         <v>0.9090909041322315</v>
       </c>
-      <c r="F146" s="9">
+      <c r="F146" s="7">
         <v>1</v>
       </c>
       <c r="G146" s="4">
         <v>0.9999996423721313</v>
       </c>
-      <c r="H146" s="9">
+      <c r="H146" s="7">
         <v>1</v>
       </c>
       <c r="I146" s="3" t="s">
@@ -18761,10 +18718,10 @@
       <c r="D156" s="4">
         <v>0.1201476976275444</v>
       </c>
-      <c r="E156" s="9">
+      <c r="E156" s="7">
         <v>0</v>
       </c>
-      <c r="F156" s="9">
+      <c r="F156" s="7">
         <v>0</v>
       </c>
       <c r="G156" s="4">
@@ -18961,19 +18918,19 @@
       <c r="C163" s="3" t="s">
         <v>498</v>
       </c>
-      <c r="D163" s="9">
+      <c r="D163" s="7">
         <v>1</v>
       </c>
       <c r="E163" s="4">
         <v>0.9230769181065088</v>
       </c>
-      <c r="F163" s="9">
+      <c r="F163" s="7">
         <v>1</v>
       </c>
       <c r="G163" s="4">
         <v>0.9999992847442627</v>
       </c>
-      <c r="H163" s="9">
+      <c r="H163" s="7">
         <v>1</v>
       </c>
       <c r="I163" s="3" t="s">
@@ -19953,7 +19910,7 @@
       <c r="E197" s="4">
         <v>0.9090909041322315</v>
       </c>
-      <c r="F197" s="9">
+      <c r="F197" s="7">
         <v>1</v>
       </c>
       <c r="G197" s="4">
@@ -20066,10 +20023,10 @@
       <c r="D201" s="4">
         <v>0.1307795643806458</v>
       </c>
-      <c r="E201" s="9">
+      <c r="E201" s="7">
         <v>0</v>
       </c>
-      <c r="F201" s="9">
+      <c r="F201" s="7">
         <v>0</v>
       </c>
       <c r="G201" s="4">
@@ -20095,10 +20052,10 @@
       <c r="D202" s="4">
         <v>0.1629054993391037</v>
       </c>
-      <c r="E202" s="9">
+      <c r="E202" s="7">
         <v>0</v>
       </c>
-      <c r="F202" s="9">
+      <c r="F202" s="7">
         <v>0</v>
       </c>
       <c r="G202" s="4">
@@ -20153,10 +20110,10 @@
       <c r="D204" s="4">
         <v>0.119794100522995</v>
       </c>
-      <c r="E204" s="9">
+      <c r="E204" s="7">
         <v>0</v>
       </c>
-      <c r="F204" s="9">
+      <c r="F204" s="7">
         <v>0</v>
       </c>
       <c r="G204" s="4">
@@ -20182,10 +20139,10 @@
       <c r="D205" s="4">
         <v>0.05591139197349548</v>
       </c>
-      <c r="E205" s="9">
+      <c r="E205" s="7">
         <v>0</v>
       </c>
-      <c r="F205" s="9">
+      <c r="F205" s="7">
         <v>0</v>
       </c>
       <c r="G205" s="4">
@@ -20211,10 +20168,10 @@
       <c r="D206" s="4">
         <v>0.1041570752859116</v>
       </c>
-      <c r="E206" s="9">
+      <c r="E206" s="7">
         <v>0</v>
       </c>
-      <c r="F206" s="9">
+      <c r="F206" s="7">
         <v>0</v>
       </c>
       <c r="G206" s="4">
@@ -20240,10 +20197,10 @@
       <c r="D207" s="4">
         <v>0.111744798719883</v>
       </c>
-      <c r="E207" s="9">
+      <c r="E207" s="7">
         <v>0</v>
       </c>
-      <c r="F207" s="9">
+      <c r="F207" s="7">
         <v>0</v>
       </c>
       <c r="G207" s="4">
@@ -20269,10 +20226,10 @@
       <c r="D208" s="4">
         <v>0.04893253743648529</v>
       </c>
-      <c r="E208" s="9">
+      <c r="E208" s="7">
         <v>0</v>
       </c>
-      <c r="F208" s="9">
+      <c r="F208" s="7">
         <v>0</v>
       </c>
       <c r="G208" s="4">
@@ -20298,10 +20255,10 @@
       <c r="D209" s="4">
         <v>0.09152138233184814</v>
       </c>
-      <c r="E209" s="9">
+      <c r="E209" s="7">
         <v>0</v>
       </c>
-      <c r="F209" s="9">
+      <c r="F209" s="7">
         <v>0</v>
       </c>
       <c r="G209" s="4">
@@ -20327,10 +20284,10 @@
       <c r="D210" s="4">
         <v>0.01734160259366035</v>
       </c>
-      <c r="E210" s="9">
+      <c r="E210" s="7">
         <v>0</v>
       </c>
-      <c r="F210" s="9">
+      <c r="F210" s="7">
         <v>0</v>
       </c>
       <c r="G210" s="4">
@@ -21200,10 +21157,10 @@
       <c r="E240" s="4">
         <v>0.9333333283555556</v>
       </c>
-      <c r="F240" s="9">
+      <c r="F240" s="7">
         <v>1</v>
       </c>
-      <c r="G240" s="9">
+      <c r="G240" s="7">
         <v>1</v>
       </c>
       <c r="H240" s="4">
@@ -21313,10 +21270,10 @@
       <c r="D244" s="4">
         <v>0.4737716913223267</v>
       </c>
-      <c r="E244" s="9">
+      <c r="E244" s="7">
         <v>0</v>
       </c>
-      <c r="F244" s="9">
+      <c r="F244" s="7">
         <v>0</v>
       </c>
       <c r="G244" s="4">
@@ -21400,10 +21357,10 @@
       <c r="D247" s="4">
         <v>-0.03720460087060928</v>
       </c>
-      <c r="E247" s="9">
+      <c r="E247" s="7">
         <v>0</v>
       </c>
-      <c r="F247" s="9">
+      <c r="F247" s="7">
         <v>0</v>
       </c>
       <c r="G247" s="4">
@@ -21519,10 +21476,10 @@
       <c r="E251" s="4">
         <v>0.959999995008</v>
       </c>
-      <c r="F251" s="9">
+      <c r="F251" s="7">
         <v>1</v>
       </c>
-      <c r="G251" s="9">
+      <c r="G251" s="7">
         <v>1</v>
       </c>
       <c r="H251" s="4">
@@ -21635,7 +21592,7 @@
       <c r="E255" s="4">
         <v>0.9473684160664821</v>
       </c>
-      <c r="F255" s="9">
+      <c r="F255" s="7">
         <v>1</v>
       </c>
       <c r="G255" s="4">
@@ -22180,7 +22137,7 @@
       <c r="C274" s="3" t="s">
         <v>826</v>
       </c>
-      <c r="D274" s="9">
+      <c r="D274" s="7">
         <v>1</v>
       </c>
       <c r="E274" s="4">
@@ -22192,7 +22149,7 @@
       <c r="G274" s="4">
         <v>0.9999992847442627</v>
       </c>
-      <c r="H274" s="9">
+      <c r="H274" s="7">
         <v>1</v>
       </c>
       <c r="I274" s="3" t="s">
@@ -22331,7 +22288,7 @@
       <c r="E279" s="4">
         <v>0.0869565175047261</v>
       </c>
-      <c r="F279" s="9">
+      <c r="F279" s="7">
         <v>0</v>
       </c>
       <c r="G279" s="4">
@@ -23607,7 +23564,7 @@
       <c r="E323" s="4">
         <v>0.9696969647015611</v>
       </c>
-      <c r="F323" s="9">
+      <c r="F323" s="7">
         <v>1</v>
       </c>
       <c r="G323" s="4">
@@ -24358,10 +24315,10 @@
       <c r="D349" s="4">
         <v>0.30490842461586</v>
       </c>
-      <c r="E349" s="9">
+      <c r="E349" s="7">
         <v>0</v>
       </c>
-      <c r="F349" s="9">
+      <c r="F349" s="7">
         <v>0</v>
       </c>
       <c r="G349" s="4">
@@ -25170,10 +25127,10 @@
       <c r="D377" s="4">
         <v>0.3447065055370331</v>
       </c>
-      <c r="E377" s="9">
+      <c r="E377" s="7">
         <v>0</v>
       </c>
-      <c r="F377" s="9">
+      <c r="F377" s="7">
         <v>0</v>
       </c>
       <c r="G377" s="4">
@@ -25637,10 +25594,10 @@
       <c r="E393" s="4">
         <v>0.9333333283555556</v>
       </c>
-      <c r="F393" s="9">
+      <c r="F393" s="7">
         <v>1</v>
       </c>
-      <c r="G393" s="9">
+      <c r="G393" s="7">
         <v>1</v>
       </c>
       <c r="H393" s="4">
@@ -26156,10 +26113,10 @@
       <c r="D411" s="4">
         <v>0.1016894653439522</v>
       </c>
-      <c r="E411" s="9">
+      <c r="E411" s="7">
         <v>0</v>
       </c>
-      <c r="F411" s="9">
+      <c r="F411" s="7">
         <v>0</v>
       </c>
       <c r="G411" s="4">
@@ -26214,10 +26171,10 @@
       <c r="D413" s="4">
         <v>0.4096655249595642</v>
       </c>
-      <c r="E413" s="9">
+      <c r="E413" s="7">
         <v>0</v>
       </c>
-      <c r="F413" s="9">
+      <c r="F413" s="7">
         <v>0</v>
       </c>
       <c r="G413" s="4">
@@ -26333,7 +26290,7 @@
       <c r="E417" s="4">
         <v>0.6666666622222223</v>
       </c>
-      <c r="F417" s="9">
+      <c r="F417" s="7">
         <v>0</v>
       </c>
       <c r="G417" s="4">
@@ -26394,7 +26351,7 @@
       <c r="F419" s="4">
         <v>1.821831989445342e-231</v>
       </c>
-      <c r="G419" s="9">
+      <c r="G419" s="7">
         <v>1</v>
       </c>
       <c r="H419" s="4">
@@ -26449,7 +26406,7 @@
       <c r="E421" s="4">
         <v>0.999999995</v>
       </c>
-      <c r="F421" s="9">
+      <c r="F421" s="7">
         <v>0</v>
       </c>
       <c r="G421" s="4">
@@ -26536,7 +26493,7 @@
       <c r="E424" s="4">
         <v>0.999999995</v>
       </c>
-      <c r="F424" s="9">
+      <c r="F424" s="7">
         <v>0</v>
       </c>
       <c r="G424" s="4">
@@ -26565,7 +26522,7 @@
       <c r="E425" s="4">
         <v>0.02631578847645433</v>
       </c>
-      <c r="F425" s="9">
+      <c r="F425" s="7">
         <v>0</v>
       </c>
       <c r="G425" s="4">
@@ -27171,10 +27128,10 @@
       <c r="D446" s="4">
         <v>0.2036039531230927</v>
       </c>
-      <c r="E446" s="9">
+      <c r="E446" s="7">
         <v>0</v>
       </c>
-      <c r="F446" s="9">
+      <c r="F446" s="7">
         <v>0</v>
       </c>
       <c r="G446" s="4">
@@ -27928,7 +27885,7 @@
       <c r="E472" s="4">
         <v>0.9090909041322315</v>
       </c>
-      <c r="F472" s="9">
+      <c r="F472" s="7">
         <v>1</v>
       </c>
       <c r="G472" s="4">
@@ -27986,7 +27943,7 @@
       <c r="E474" s="4">
         <v>0.07999999852800002</v>
       </c>
-      <c r="F474" s="9">
+      <c r="F474" s="7">
         <v>0</v>
       </c>
       <c r="G474" s="4">
@@ -28215,10 +28172,10 @@
       <c r="D482" s="4">
         <v>0.2853322327136993</v>
       </c>
-      <c r="E482" s="9">
+      <c r="E482" s="7">
         <v>0</v>
       </c>
-      <c r="F482" s="9">
+      <c r="F482" s="7">
         <v>0</v>
       </c>
       <c r="G482" s="4">
@@ -28624,7 +28581,7 @@
       <c r="E496" s="4">
         <v>0.9333333283555556</v>
       </c>
-      <c r="F496" s="9">
+      <c r="F496" s="7">
         <v>1</v>
       </c>
       <c r="G496" s="4">
@@ -28969,10 +28926,10 @@
       <c r="D508" s="4">
         <v>0.1997150033712387</v>
       </c>
-      <c r="E508" s="9">
+      <c r="E508" s="7">
         <v>0</v>
       </c>
-      <c r="F508" s="9">
+      <c r="F508" s="7">
         <v>0</v>
       </c>
       <c r="G508" s="4">
@@ -29314,19 +29271,19 @@
       <c r="C520" s="3" t="s">
         <v>1564</v>
       </c>
-      <c r="D520" s="9">
+      <c r="D520" s="7">
         <v>1</v>
       </c>
       <c r="E520" s="4">
         <v>0.9473684160664821</v>
       </c>
-      <c r="F520" s="9">
+      <c r="F520" s="7">
         <v>1</v>
       </c>
-      <c r="G520" s="9">
+      <c r="G520" s="7">
         <v>1</v>
       </c>
-      <c r="H520" s="9">
+      <c r="H520" s="7">
         <v>1</v>
       </c>
       <c r="I520" s="3" t="s">
@@ -29520,10 +29477,10 @@
       <c r="D527" s="4">
         <v>0.03364903852343559</v>
       </c>
-      <c r="E527" s="9">
+      <c r="E527" s="7">
         <v>0</v>
       </c>
-      <c r="F527" s="9">
+      <c r="F527" s="7">
         <v>0</v>
       </c>
       <c r="G527" s="4">
@@ -30071,10 +30028,10 @@
       <c r="D546" s="4">
         <v>0.3961167335510254</v>
       </c>
-      <c r="E546" s="9">
+      <c r="E546" s="7">
         <v>0</v>
       </c>
-      <c r="F546" s="9">
+      <c r="F546" s="7">
         <v>0</v>
       </c>
       <c r="G546" s="4">
@@ -30097,19 +30054,19 @@
       <c r="C547" s="3" t="s">
         <v>1644</v>
       </c>
-      <c r="D547" s="9">
+      <c r="D547" s="7">
         <v>1</v>
       </c>
       <c r="E547" s="4">
         <v>0.9230769181065088</v>
       </c>
-      <c r="F547" s="9">
+      <c r="F547" s="7">
         <v>1</v>
       </c>
-      <c r="G547" s="9">
+      <c r="G547" s="7">
         <v>1</v>
       </c>
-      <c r="H547" s="9">
+      <c r="H547" s="7">
         <v>1</v>
       </c>
       <c r="I547" s="3" t="s">
@@ -30416,19 +30373,19 @@
       <c r="C558" s="3" t="s">
         <v>1677</v>
       </c>
-      <c r="D558" s="9">
+      <c r="D558" s="7">
         <v>1</v>
       </c>
       <c r="E558" s="4">
         <v>0.9411764656055364</v>
       </c>
-      <c r="F558" s="9">
+      <c r="F558" s="7">
         <v>1</v>
       </c>
-      <c r="G558" s="9">
+      <c r="G558" s="7">
         <v>1</v>
       </c>
-      <c r="H558" s="9">
+      <c r="H558" s="7">
         <v>1</v>
       </c>
       <c r="I558" s="3" t="s">
@@ -30767,10 +30724,10 @@
       <c r="D570" s="4">
         <v>0.2658750414848328</v>
       </c>
-      <c r="E570" s="9">
+      <c r="E570" s="7">
         <v>0</v>
       </c>
-      <c r="F570" s="9">
+      <c r="F570" s="7">
         <v>0</v>
       </c>
       <c r="G570" s="4">
@@ -32539,7 +32496,7 @@
       <c r="E631" s="4">
         <v>0.04999999820000006</v>
       </c>
-      <c r="F631" s="9">
+      <c r="F631" s="7">
         <v>0</v>
       </c>
       <c r="G631" s="4">
@@ -32858,7 +32815,7 @@
       <c r="E642" s="4">
         <v>0.04545454082644675</v>
       </c>
-      <c r="F642" s="9">
+      <c r="F642" s="7">
         <v>0</v>
       </c>
       <c r="G642" s="4">
@@ -35004,10 +34961,10 @@
       <c r="E716" s="4">
         <v>0.9333333283555556</v>
       </c>
-      <c r="F716" s="9">
+      <c r="F716" s="7">
         <v>1</v>
       </c>
-      <c r="G716" s="9">
+      <c r="G716" s="7">
         <v>1</v>
       </c>
       <c r="H716" s="4">
@@ -35027,19 +34984,19 @@
       <c r="C717" s="3" t="s">
         <v>2153</v>
       </c>
-      <c r="D717" s="9">
+      <c r="D717" s="7">
         <v>1</v>
       </c>
       <c r="E717" s="4">
         <v>0.9333333283555556</v>
       </c>
-      <c r="F717" s="9">
+      <c r="F717" s="7">
         <v>1</v>
       </c>
-      <c r="G717" s="9">
+      <c r="G717" s="7">
         <v>1</v>
       </c>
-      <c r="H717" s="9">
+      <c r="H717" s="7">
         <v>1</v>
       </c>
       <c r="I717" s="3" t="s">
@@ -35175,10 +35132,10 @@
       <c r="D722" s="4">
         <v>0.6097208261489868</v>
       </c>
-      <c r="E722" s="9">
+      <c r="E722" s="7">
         <v>0</v>
       </c>
-      <c r="F722" s="9">
+      <c r="F722" s="7">
         <v>0</v>
       </c>
       <c r="G722" s="4">
@@ -36541,10 +36498,10 @@
       <c r="E769" s="4">
         <v>0.9090909041322315</v>
       </c>
-      <c r="F769" s="9">
+      <c r="F769" s="7">
         <v>1</v>
       </c>
-      <c r="G769" s="9">
+      <c r="G769" s="7">
         <v>1</v>
       </c>
       <c r="H769" s="4">
@@ -36741,10 +36698,10 @@
       <c r="D776" s="4">
         <v>0.229666993021965</v>
       </c>
-      <c r="E776" s="9">
+      <c r="E776" s="7">
         <v>0</v>
       </c>
-      <c r="F776" s="9">
+      <c r="F776" s="7">
         <v>0</v>
       </c>
       <c r="G776" s="4">
@@ -38281,7 +38238,7 @@
       <c r="E829" s="4">
         <v>0.1538461524260355</v>
       </c>
-      <c r="F829" s="9">
+      <c r="F829" s="7">
         <v>0</v>
       </c>
       <c r="G829" s="4">
@@ -38571,10 +38528,10 @@
       <c r="E839" s="4">
         <v>0.959999995008</v>
       </c>
-      <c r="F839" s="9">
+      <c r="F839" s="7">
         <v>1</v>
       </c>
-      <c r="G839" s="9">
+      <c r="G839" s="7">
         <v>1</v>
       </c>
       <c r="H839" s="4">
@@ -39322,10 +39279,10 @@
       <c r="D865" s="4">
         <v>0.4395512342453003</v>
       </c>
-      <c r="E865" s="9">
+      <c r="E865" s="7">
         <v>0</v>
       </c>
-      <c r="F865" s="9">
+      <c r="F865" s="7">
         <v>0</v>
       </c>
       <c r="G865" s="4">
@@ -39464,7 +39421,7 @@
       <c r="C870" s="3" t="s">
         <v>2608</v>
       </c>
-      <c r="D870" s="9">
+      <c r="D870" s="7">
         <v>1</v>
       </c>
       <c r="E870" s="4">
@@ -39476,7 +39433,7 @@
       <c r="G870" s="4">
         <v>1.000001430511475</v>
       </c>
-      <c r="H870" s="9">
+      <c r="H870" s="7">
         <v>1</v>
       </c>
       <c r="I870" s="3" t="s">
@@ -39525,10 +39482,10 @@
       <c r="D872" s="4">
         <v>0.5049467086791992</v>
       </c>
-      <c r="E872" s="9">
+      <c r="E872" s="7">
         <v>0</v>
       </c>
-      <c r="F872" s="9">
+      <c r="F872" s="7">
         <v>0</v>
       </c>
       <c r="G872" s="4">
@@ -39757,10 +39714,10 @@
       <c r="D880" s="4">
         <v>0.4386080205440521</v>
       </c>
-      <c r="E880" s="9">
+      <c r="E880" s="7">
         <v>0</v>
       </c>
-      <c r="F880" s="9">
+      <c r="F880" s="7">
         <v>0</v>
       </c>
       <c r="G880" s="4">
@@ -42225,7 +42182,7 @@
       <c r="E965" s="4">
         <v>0.06666666202222254</v>
       </c>
-      <c r="F965" s="9">
+      <c r="F965" s="7">
         <v>0</v>
       </c>
       <c r="G965" s="4">
@@ -42628,10 +42585,10 @@
       <c r="D979" s="4">
         <v>0.02800870127975941</v>
       </c>
-      <c r="E979" s="9">
+      <c r="E979" s="7">
         <v>0</v>
       </c>
-      <c r="F979" s="9">
+      <c r="F979" s="7">
         <v>0</v>
       </c>
       <c r="G979" s="4">
@@ -42689,7 +42646,7 @@
       <c r="E981" s="4">
         <v>0.08695652015122875</v>
       </c>
-      <c r="F981" s="9">
+      <c r="F981" s="7">
         <v>0</v>
       </c>
       <c r="G981" s="4">
@@ -42799,7 +42756,7 @@
       <c r="C985" s="3" t="s">
         <v>2945</v>
       </c>
-      <c r="D985" s="9">
+      <c r="D985" s="7">
         <v>1</v>
       </c>
       <c r="E985" s="4">
@@ -42811,7 +42768,7 @@
       <c r="G985" s="4">
         <v>1.000000715255737</v>
       </c>
-      <c r="H985" s="9">
+      <c r="H985" s="7">
         <v>1</v>
       </c>
       <c r="I985" s="3" t="s">
@@ -43150,10 +43107,10 @@
       <c r="D997" s="4">
         <v>0.7422190308570862</v>
       </c>
-      <c r="E997" s="9">
+      <c r="E997" s="7">
         <v>0</v>
       </c>
-      <c r="F997" s="9">
+      <c r="F997" s="7">
         <v>0</v>
       </c>
       <c r="G997" s="4">
@@ -43994,7 +43951,7 @@
       <c r="E1026" s="4">
         <v>0.999999995</v>
       </c>
-      <c r="F1026" s="9">
+      <c r="F1026" s="7">
         <v>0</v>
       </c>
       <c r="G1026" s="4">
@@ -44023,7 +43980,7 @@
       <c r="E1027" s="4">
         <v>0.1999999968</v>
       </c>
-      <c r="F1027" s="9">
+      <c r="F1027" s="7">
         <v>0</v>
       </c>
       <c r="G1027" s="4">
@@ -44046,7 +44003,7 @@
       <c r="C1028" s="3" t="s">
         <v>3059</v>
       </c>
-      <c r="D1028" s="9">
+      <c r="D1028" s="7">
         <v>1</v>
       </c>
       <c r="E1028" s="4">
@@ -44055,10 +44012,10 @@
       <c r="F1028" s="4">
         <v>1.491668146240062e-154</v>
       </c>
-      <c r="G1028" s="9">
+      <c r="G1028" s="7">
         <v>1</v>
       </c>
-      <c r="H1028" s="9">
+      <c r="H1028" s="7">
         <v>1</v>
       </c>
       <c r="I1028" s="3" t="s">
@@ -44107,10 +44064,10 @@
       <c r="D1030" s="4">
         <v>0.6349645853042603</v>
       </c>
-      <c r="E1030" s="9">
+      <c r="E1030" s="7">
         <v>0</v>
       </c>
-      <c r="F1030" s="9">
+      <c r="F1030" s="7">
         <v>0</v>
       </c>
       <c r="G1030" s="4">
@@ -44139,7 +44096,7 @@
       <c r="E1031" s="4">
         <v>0.999999995</v>
       </c>
-      <c r="F1031" s="9">
+      <c r="F1031" s="7">
         <v>0</v>
       </c>
       <c r="G1031" s="4">
@@ -45386,7 +45343,7 @@
       <c r="E1074" s="4">
         <v>0.04444443950617339</v>
       </c>
-      <c r="F1074" s="9">
+      <c r="F1074" s="7">
         <v>0</v>
       </c>
       <c r="G1074" s="4">
@@ -45412,10 +45369,10 @@
       <c r="D1075" s="4">
         <v>0.04604204744100571</v>
       </c>
-      <c r="E1075" s="9">
+      <c r="E1075" s="7">
         <v>0</v>
       </c>
-      <c r="F1075" s="9">
+      <c r="F1075" s="7">
         <v>0</v>
       </c>
       <c r="G1075" s="4">
@@ -45470,10 +45427,10 @@
       <c r="D1077" s="4">
         <v>0.02355531603097916</v>
       </c>
-      <c r="E1077" s="9">
+      <c r="E1077" s="7">
         <v>0</v>
       </c>
-      <c r="F1077" s="9">
+      <c r="F1077" s="7">
         <v>0</v>
       </c>
       <c r="G1077" s="4">
@@ -45528,10 +45485,10 @@
       <c r="D1079" s="4">
         <v>0.04228588193655014</v>
       </c>
-      <c r="E1079" s="9">
+      <c r="E1079" s="7">
         <v>0</v>
       </c>
-      <c r="F1079" s="9">
+      <c r="F1079" s="7">
         <v>0</v>
       </c>
       <c r="G1079" s="4">
@@ -45560,7 +45517,7 @@
       <c r="E1080" s="4">
         <v>0.02941176285899666</v>
       </c>
-      <c r="F1080" s="9">
+      <c r="F1080" s="7">
         <v>0</v>
       </c>
       <c r="G1080" s="4">
@@ -47387,7 +47344,7 @@
       <c r="E1143" s="4">
         <v>0.2857142832653061</v>
       </c>
-      <c r="F1143" s="9">
+      <c r="F1143" s="7">
         <v>0</v>
       </c>
       <c r="G1143" s="4">
@@ -47558,10 +47515,10 @@
       <c r="D1149" s="4">
         <v>0.3176071345806122</v>
       </c>
-      <c r="E1149" s="9">
+      <c r="E1149" s="7">
         <v>0</v>
       </c>
-      <c r="F1149" s="9">
+      <c r="F1149" s="7">
         <v>0</v>
       </c>
       <c r="G1149" s="4">
@@ -47587,10 +47544,10 @@
       <c r="D1150" s="4">
         <v>0.7555330395698547</v>
       </c>
-      <c r="E1150" s="9">
+      <c r="E1150" s="7">
         <v>0</v>
       </c>
-      <c r="F1150" s="9">
+      <c r="F1150" s="7">
         <v>0</v>
       </c>
       <c r="G1150" s="4">
@@ -47674,10 +47631,10 @@
       <c r="D1153" s="4">
         <v>0.0152645343914628</v>
       </c>
-      <c r="E1153" s="9">
+      <c r="E1153" s="7">
         <v>0</v>
       </c>
-      <c r="F1153" s="9">
+      <c r="F1153" s="7">
         <v>0</v>
       </c>
       <c r="G1153" s="4">
@@ -47848,10 +47805,10 @@
       <c r="D1159" s="4">
         <v>0.4656542539596558</v>
       </c>
-      <c r="E1159" s="9">
+      <c r="E1159" s="7">
         <v>0</v>
       </c>
-      <c r="F1159" s="9">
+      <c r="F1159" s="7">
         <v>0</v>
       </c>
       <c r="G1159" s="4">
@@ -48544,10 +48501,10 @@
       <c r="D1183" s="4">
         <v>0.4510446488857269</v>
       </c>
-      <c r="E1183" s="9">
+      <c r="E1183" s="7">
         <v>0</v>
       </c>
-      <c r="F1183" s="9">
+      <c r="F1183" s="7">
         <v>0</v>
       </c>
       <c r="G1183" s="4">
@@ -50313,10 +50270,10 @@
       <c r="D1244" s="4">
         <v>0.6284278631210327</v>
       </c>
-      <c r="E1244" s="9">
+      <c r="E1244" s="7">
         <v>0</v>
       </c>
-      <c r="F1244" s="9">
+      <c r="F1244" s="7">
         <v>0</v>
       </c>
       <c r="G1244" s="4">
@@ -51299,10 +51256,10 @@
       <c r="D1278" s="4">
         <v>0.3830941021442413</v>
       </c>
-      <c r="E1278" s="9">
+      <c r="E1278" s="7">
         <v>0</v>
       </c>
-      <c r="F1278" s="9">
+      <c r="F1278" s="7">
         <v>0</v>
       </c>
       <c r="G1278" s="4">
@@ -52839,7 +52796,7 @@
       <c r="E1331" s="4">
         <v>0.999999995</v>
       </c>
-      <c r="F1331" s="9">
+      <c r="F1331" s="7">
         <v>1</v>
       </c>
       <c r="G1331" s="4">
@@ -52921,19 +52878,19 @@
         <v>3972</v>
       </c>
       <c r="D1334" s="4">
-        <v>-0.06195624172687531</v>
+        <v>0.3120104074478149</v>
       </c>
       <c r="E1334" s="4">
-        <v>0.02739725790955172</v>
+        <v>0.06249999517578163</v>
       </c>
       <c r="F1334" s="4">
-        <v>6.254249455964533e-232</v>
+        <v>5.025547213910947e-232</v>
       </c>
       <c r="G1334" s="4">
-        <v>-0.1920593678951263</v>
+        <v>0.0765082985162735</v>
       </c>
       <c r="H1334" s="4">
-        <v>-0.06195624172687531</v>
+        <v>0.3120104074478149</v>
       </c>
       <c r="I1334" s="3" t="s">
         <v>21</v>
@@ -52950,19 +52907,19 @@
         <v>3975</v>
       </c>
       <c r="D1335" s="4">
-        <v>0.3120104074478149</v>
+        <v>0.4342172145843506</v>
       </c>
       <c r="E1335" s="4">
-        <v>0.06249999517578163</v>
+        <v>0.08333333003472235</v>
       </c>
       <c r="F1335" s="4">
-        <v>5.025547213910947e-232</v>
+        <v>3.197364103008188e-233</v>
       </c>
       <c r="G1335" s="4">
-        <v>0.0765082985162735</v>
+        <v>0.1337480843067169</v>
       </c>
       <c r="H1335" s="4">
-        <v>0.3120104074478149</v>
+        <v>0.4342172145843506</v>
       </c>
       <c r="I1335" s="3" t="s">
         <v>21</v>
@@ -52976,54 +52933,54 @@
         <v>3977</v>
       </c>
       <c r="C1336" s="3" t="s">
-        <v>3978</v>
+        <v>3977</v>
       </c>
       <c r="D1336" s="4">
-        <v>0.4342172145843506</v>
+        <v>1.00000011920929</v>
       </c>
       <c r="E1336" s="4">
-        <v>0.08333333003472235</v>
-      </c>
-      <c r="F1336" s="4">
-        <v>3.197364103008188e-233</v>
-      </c>
-      <c r="G1336" s="4">
-        <v>0.1337480843067169</v>
+        <v>0.999999995</v>
+      </c>
+      <c r="F1336" s="7">
+        <v>1</v>
+      </c>
+      <c r="G1336" s="7">
+        <v>1</v>
       </c>
       <c r="H1336" s="4">
-        <v>0.4342172145843506</v>
+        <v>1.00000011920929</v>
       </c>
       <c r="I1336" s="3" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="1337" customHeight="1" ht="16.5">
       <c r="A1337" s="3" t="s">
+        <v>3978</v>
+      </c>
+      <c r="B1337" s="3" t="s">
         <v>3979</v>
-      </c>
-      <c r="B1337" s="3" t="s">
-        <v>3980</v>
       </c>
       <c r="C1337" s="3" t="s">
         <v>3980</v>
       </c>
       <c r="D1337" s="4">
-        <v>1.00000011920929</v>
+        <v>0.3580803573131561</v>
       </c>
       <c r="E1337" s="4">
-        <v>0.999999995</v>
-      </c>
-      <c r="F1337" s="9">
-        <v>1</v>
-      </c>
-      <c r="G1337" s="9">
-        <v>1</v>
+        <v>0.03508771618344134</v>
+      </c>
+      <c r="F1337" s="7">
+        <v>0</v>
+      </c>
+      <c r="G1337" s="4">
+        <v>0.1941829323768616</v>
       </c>
       <c r="H1337" s="4">
-        <v>1.00000011920929</v>
+        <v>0.3580803573131561</v>
       </c>
       <c r="I1337" s="3" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="1338" customHeight="1" ht="16.5">
@@ -53037,19 +52994,19 @@
         <v>3983</v>
       </c>
       <c r="D1338" s="4">
-        <v>0.3580803573131561</v>
+        <v>0.3340105414390564</v>
       </c>
       <c r="E1338" s="4">
-        <v>0.03508771618344134</v>
-      </c>
-      <c r="F1338" s="9">
-        <v>0</v>
+        <v>0.1132075426842294</v>
+      </c>
+      <c r="F1338" s="4">
+        <v>9.418382295637229e-232</v>
       </c>
       <c r="G1338" s="4">
-        <v>0.1941829323768616</v>
+        <v>0.1095720306038857</v>
       </c>
       <c r="H1338" s="4">
-        <v>0.3580803573131561</v>
+        <v>0.3340105414390564</v>
       </c>
       <c r="I1338" s="3" t="s">
         <v>21</v>
@@ -53066,19 +53023,19 @@
         <v>3986</v>
       </c>
       <c r="D1339" s="4">
-        <v>0.3340105414390564</v>
+        <v>0.1713999956846237</v>
       </c>
       <c r="E1339" s="4">
-        <v>0.1132075426842294</v>
+        <v>0.04878048316478331</v>
       </c>
       <c r="F1339" s="4">
-        <v>9.418382295637229e-232</v>
+        <v>9.594503055152632e-232</v>
       </c>
       <c r="G1339" s="4">
-        <v>0.1095720306038857</v>
+        <v>0.05252471938729286</v>
       </c>
       <c r="H1339" s="4">
-        <v>0.3340105414390564</v>
+        <v>0.1713999956846237</v>
       </c>
       <c r="I1339" s="3" t="s">
         <v>21</v>
@@ -53095,19 +53052,19 @@
         <v>3989</v>
       </c>
       <c r="D1340" s="4">
-        <v>0.1713999956846237</v>
+        <v>0.2408482730388641</v>
       </c>
       <c r="E1340" s="4">
-        <v>0.04878048316478331</v>
+        <v>0.1333333284543212</v>
       </c>
       <c r="F1340" s="4">
-        <v>9.594503055152632e-232</v>
+        <v>8.416851712392762e-232</v>
       </c>
       <c r="G1340" s="4">
-        <v>0.05252471938729286</v>
+        <v>0.07979588955640793</v>
       </c>
       <c r="H1340" s="4">
-        <v>0.1713999956846237</v>
+        <v>0.2408482730388641</v>
       </c>
       <c r="I1340" s="3" t="s">
         <v>21</v>
@@ -53124,19 +53081,19 @@
         <v>3992</v>
       </c>
       <c r="D1341" s="4">
-        <v>0.2408482730388641</v>
+        <v>0.09777110069990158</v>
       </c>
       <c r="E1341" s="4">
-        <v>0.1333333284543212</v>
+        <v>0.09523809069286994</v>
       </c>
       <c r="F1341" s="4">
-        <v>8.416851712392762e-232</v>
+        <v>8.726094729337945e-232</v>
       </c>
       <c r="G1341" s="4">
-        <v>0.07979588955640793</v>
+        <v>0.07483290135860443</v>
       </c>
       <c r="H1341" s="4">
-        <v>0.2408482730388641</v>
+        <v>0.09777110069990158</v>
       </c>
       <c r="I1341" s="3" t="s">
         <v>21</v>
@@ -53153,19 +53110,19 @@
         <v>3995</v>
       </c>
       <c r="D1342" s="4">
-        <v>0.09777110069990158</v>
+        <v>-0.00395321287214756</v>
       </c>
       <c r="E1342" s="4">
-        <v>0.09523809069286994</v>
+        <v>0.05063290761096007</v>
       </c>
       <c r="F1342" s="4">
-        <v>8.726094729337945e-232</v>
+        <v>8.81439698262975e-232</v>
       </c>
       <c r="G1342" s="4">
-        <v>0.07483290135860443</v>
+        <v>0.01418792922049761</v>
       </c>
       <c r="H1342" s="4">
-        <v>0.09777110069990158</v>
+        <v>-0.00395321287214756</v>
       </c>
       <c r="I1342" s="3" t="s">
         <v>21</v>
@@ -53182,19 +53139,19 @@
         <v>3998</v>
       </c>
       <c r="D1343" s="4">
-        <v>-0.00395321287214756</v>
+        <v>0.04417499527335167</v>
       </c>
       <c r="E1343" s="4">
-        <v>0.05063290761096007</v>
+        <v>0.1714285665306124</v>
       </c>
       <c r="F1343" s="4">
-        <v>8.81439698262975e-232</v>
+        <v>9.380709333728914e-232</v>
       </c>
       <c r="G1343" s="4">
-        <v>0.01418792922049761</v>
+        <v>0.07833803445100784</v>
       </c>
       <c r="H1343" s="4">
-        <v>-0.00395321287214756</v>
+        <v>0.04417499527335167</v>
       </c>
       <c r="I1343" s="3" t="s">
         <v>21</v>
@@ -53211,19 +53168,19 @@
         <v>4001</v>
       </c>
       <c r="D1344" s="4">
-        <v>0.04417499527335167</v>
+        <v>0.09475906938314438</v>
       </c>
       <c r="E1344" s="4">
-        <v>0.1714285665306124</v>
+        <v>0.1538461488535504</v>
       </c>
       <c r="F1344" s="4">
-        <v>9.380709333728914e-232</v>
+        <v>1.110257771799128e-231</v>
       </c>
       <c r="G1344" s="4">
-        <v>0.07833803445100784</v>
+        <v>0.0428466685116291</v>
       </c>
       <c r="H1344" s="4">
-        <v>0.04417499527335167</v>
+        <v>0.09475906938314438</v>
       </c>
       <c r="I1344" s="3" t="s">
         <v>21</v>
@@ -53240,19 +53197,19 @@
         <v>4004</v>
       </c>
       <c r="D1345" s="4">
-        <v>0.09475906938314438</v>
+        <v>0.04368384182453156</v>
       </c>
       <c r="E1345" s="4">
-        <v>0.1538461488535504</v>
+        <v>0.0952380902380955</v>
       </c>
       <c r="F1345" s="4">
-        <v>1.110257771799128e-231</v>
+        <v>1.012071042130996e-231</v>
       </c>
       <c r="G1345" s="4">
-        <v>0.0428466685116291</v>
+        <v>0.0272609256207943</v>
       </c>
       <c r="H1345" s="4">
-        <v>0.09475906938314438</v>
+        <v>0.04368384182453156</v>
       </c>
       <c r="I1345" s="3" t="s">
         <v>21</v>
@@ -53269,19 +53226,19 @@
         <v>4007</v>
       </c>
       <c r="D1346" s="4">
-        <v>0.04368384182453156</v>
+        <v>0.3548681437969208</v>
       </c>
       <c r="E1346" s="4">
-        <v>0.0952380902380955</v>
+        <v>0.03225806120187339</v>
       </c>
       <c r="F1346" s="4">
-        <v>1.012071042130996e-231</v>
+        <v>6.573479617511883e-232</v>
       </c>
       <c r="G1346" s="4">
-        <v>0.0272609256207943</v>
+        <v>0.03638098016381264</v>
       </c>
       <c r="H1346" s="4">
-        <v>0.04368384182453156</v>
+        <v>0.3548681437969208</v>
       </c>
       <c r="I1346" s="3" t="s">
         <v>21</v>
@@ -53298,19 +53255,19 @@
         <v>4010</v>
       </c>
       <c r="D1347" s="4">
-        <v>0.3548681437969208</v>
+        <v>0.1954070031642914</v>
       </c>
       <c r="E1347" s="4">
-        <v>0.03225806120187339</v>
+        <v>0.03448275514268763</v>
       </c>
       <c r="F1347" s="4">
-        <v>6.573479617511883e-232</v>
+        <v>6.784338172413661e-232</v>
       </c>
       <c r="G1347" s="4">
-        <v>0.03638098016381264</v>
+        <v>0.08902966231107712</v>
       </c>
       <c r="H1347" s="4">
-        <v>0.3548681437969208</v>
+        <v>0.1954070031642914</v>
       </c>
       <c r="I1347" s="3" t="s">
         <v>21</v>
@@ -53327,19 +53284,19 @@
         <v>4013</v>
       </c>
       <c r="D1348" s="4">
-        <v>0.1954070031642914</v>
+        <v>0.3926132619380951</v>
       </c>
       <c r="E1348" s="4">
-        <v>0.03448275514268763</v>
+        <v>0.1190476159637189</v>
       </c>
       <c r="F1348" s="4">
-        <v>6.784338172413661e-232</v>
+        <v>9.109159947227211e-232</v>
       </c>
       <c r="G1348" s="4">
-        <v>0.08902966231107712</v>
+        <v>0.1050035282969475</v>
       </c>
       <c r="H1348" s="4">
-        <v>0.1954070031642914</v>
+        <v>0.3926132619380951</v>
       </c>
       <c r="I1348" s="3" t="s">
         <v>21</v>
@@ -53356,19 +53313,19 @@
         <v>4016</v>
       </c>
       <c r="D1349" s="4">
-        <v>0.3926132619380951</v>
+        <v>0.39849653840065</v>
       </c>
       <c r="E1349" s="4">
-        <v>0.1190476159637189</v>
+        <v>0.07017543455832588</v>
       </c>
       <c r="F1349" s="4">
-        <v>9.109159947227211e-232</v>
+        <v>9.157231061812019e-232</v>
       </c>
       <c r="G1349" s="4">
-        <v>0.1050035282969475</v>
+        <v>0.1531236171722412</v>
       </c>
       <c r="H1349" s="4">
-        <v>0.3926132619380951</v>
+        <v>0.39849653840065</v>
       </c>
       <c r="I1349" s="3" t="s">
         <v>21</v>
@@ -53385,19 +53342,19 @@
         <v>4019</v>
       </c>
       <c r="D1350" s="4">
-        <v>0.39849653840065</v>
+        <v>0.1601637899875641</v>
       </c>
       <c r="E1350" s="4">
-        <v>0.07017543455832588</v>
+        <v>0.02816901091846892</v>
       </c>
       <c r="F1350" s="4">
-        <v>9.157231061812019e-232</v>
+        <v>6.391787670555036e-232</v>
       </c>
       <c r="G1350" s="4">
-        <v>0.1531236171722412</v>
+        <v>0.01010820176452398</v>
       </c>
       <c r="H1350" s="4">
-        <v>0.39849653840065</v>
+        <v>0.1601637899875641</v>
       </c>
       <c r="I1350" s="3" t="s">
         <v>21</v>
@@ -53414,19 +53371,19 @@
         <v>4022</v>
       </c>
       <c r="D1351" s="4">
-        <v>0.1601637899875641</v>
+        <v>0.3556978404521942</v>
       </c>
       <c r="E1351" s="4">
-        <v>0.02816901091846892</v>
+        <v>0.1558441522617643</v>
       </c>
       <c r="F1351" s="4">
-        <v>6.391787670555036e-232</v>
+        <v>2.66921741036689e-155</v>
       </c>
       <c r="G1351" s="4">
-        <v>0.01010820176452398</v>
+        <v>0.1845133602619171</v>
       </c>
       <c r="H1351" s="4">
-        <v>0.1601637899875641</v>
+        <v>0.3556978404521942</v>
       </c>
       <c r="I1351" s="3" t="s">
         <v>21</v>
@@ -53443,50 +53400,21 @@
         <v>4025</v>
       </c>
       <c r="D1352" s="4">
-        <v>0.3556978404521942</v>
+        <v>0.3389920294284821</v>
       </c>
       <c r="E1352" s="4">
-        <v>0.1558441522617643</v>
+        <v>0.1311475371136792</v>
       </c>
       <c r="F1352" s="4">
-        <v>2.66921741036689e-155</v>
+        <v>9.5489221792564e-232</v>
       </c>
       <c r="G1352" s="4">
-        <v>0.1845133602619171</v>
+        <v>0.1222318261861801</v>
       </c>
       <c r="H1352" s="4">
-        <v>0.3556978404521942</v>
+        <v>0.3389920294284821</v>
       </c>
       <c r="I1352" s="3" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="1353" customHeight="1" ht="16.5">
-      <c r="A1353" s="3" t="s">
-        <v>4026</v>
-      </c>
-      <c r="B1353" s="3" t="s">
-        <v>4027</v>
-      </c>
-      <c r="C1353" s="3" t="s">
-        <v>4028</v>
-      </c>
-      <c r="D1353" s="4">
-        <v>0.3389920294284821</v>
-      </c>
-      <c r="E1353" s="4">
-        <v>0.1311475371136792</v>
-      </c>
-      <c r="F1353" s="4">
-        <v>9.5489221792564e-232</v>
-      </c>
-      <c r="G1353" s="4">
-        <v>0.1222318261861801</v>
-      </c>
-      <c r="H1353" s="4">
-        <v>0.3389920294284821</v>
-      </c>
-      <c r="I1353" s="3" t="s">
         <v>21</v>
       </c>
     </row>

</xml_diff>